<commit_message>
"Updated Progres Monitoring.xlsx template"
</commit_message>
<xml_diff>
--- a/public/templates/Progres Monitoring.xlsx
+++ b/public/templates/Progres Monitoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Laravel Project/SiAPP Transda v2/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3548D063-3B32-D84A-97CE-980A1039D5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F5AE83-041D-1C48-94A7-ADD49578C592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="16360" xr2:uid="{6B4B9E33-E84D-4640-924B-8C61723094C8}"/>
   </bookViews>
@@ -192,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +203,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -307,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -343,23 +349,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -776,7 +788,9 @@
   </sheetPr>
   <dimension ref="A1:AE998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q31" workbookViewId="0">
+      <selection activeCell="AA35" sqref="AA35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -807,38 +821,38 @@
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="17" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="19" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="17" t="s">
+      <c r="K5" s="21"/>
+      <c r="L5" s="19" t="s">
         <v>14</v>
       </c>
       <c r="M5" s="20"/>
       <c r="N5" s="20"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="17" t="s">
+      <c r="O5" s="21"/>
+      <c r="P5" s="19" t="s">
         <v>13</v>
       </c>
       <c r="Q5" s="20"/>
@@ -849,89 +863,89 @@
       <c r="V5" s="20"/>
       <c r="W5" s="20"/>
       <c r="X5" s="20"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="17" t="s">
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="17" t="s">
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AE5" s="18"/>
+      <c r="AE5" s="21"/>
     </row>
     <row r="6" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="15" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="21"/>
+      <c r="J6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="17" t="s">
+      <c r="K6" s="21"/>
+      <c r="L6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="18"/>
-      <c r="N6" s="17" t="s">
+      <c r="M6" s="21"/>
+      <c r="N6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="17" t="s">
+      <c r="O6" s="21"/>
+      <c r="P6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="17" t="s">
+      <c r="Q6" s="21"/>
+      <c r="R6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="18"/>
-      <c r="T6" s="17" t="s">
+      <c r="S6" s="21"/>
+      <c r="T6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="U6" s="18"/>
-      <c r="V6" s="17" t="s">
+      <c r="U6" s="21"/>
+      <c r="V6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="W6" s="18"/>
-      <c r="X6" s="17" t="s">
+      <c r="W6" s="21"/>
+      <c r="X6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="17" t="s">
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="17" t="s">
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="15" t="s">
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AE6" s="15" t="s">
+      <c r="AE6" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="6" t="s">
         <v>5</v>
       </c>
@@ -998,8 +1012,8 @@
       <c r="AC7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="16"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
     </row>
     <row r="8" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
@@ -1113,91 +1127,91 @@
         <f>AVERAGE(G9,I9,K9,M9,O9,Q9,S9,U9,W9,Y9,AA9,AC9,AE9)</f>
         <v>1.1538461538461536E-2</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="15">
         <v>0.3</v>
       </c>
       <c r="G9" s="13">
         <f>F9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="15">
         <v>0.3</v>
       </c>
       <c r="I9" s="13">
-        <f t="shared" ref="I9:AE9" si="0">H9/$D9</f>
+        <f t="shared" ref="I9" si="0">H9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="15">
         <v>0.3</v>
       </c>
       <c r="K9" s="13">
-        <f t="shared" ref="K9:AE9" si="1">J9/$D9</f>
+        <f t="shared" ref="K9" si="1">J9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="15">
         <v>0.3</v>
       </c>
       <c r="M9" s="13">
-        <f t="shared" ref="M9:AE9" si="2">L9/$D9</f>
+        <f t="shared" ref="M9" si="2">L9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="15">
         <v>0.3</v>
       </c>
       <c r="O9" s="13">
-        <f t="shared" ref="O9:AE9" si="3">N9/$D9</f>
+        <f t="shared" ref="O9" si="3">N9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="P9" s="23">
+      <c r="P9" s="15">
         <v>0.3</v>
       </c>
       <c r="Q9" s="13">
-        <f t="shared" ref="Q9:AE9" si="4">P9/$D9</f>
+        <f t="shared" ref="Q9" si="4">P9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="R9" s="23">
+      <c r="R9" s="15">
         <v>0.3</v>
       </c>
       <c r="S9" s="13">
-        <f t="shared" ref="S9:AE9" si="5">R9/$D9</f>
+        <f t="shared" ref="S9" si="5">R9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="T9" s="23">
+      <c r="T9" s="15">
         <v>0.3</v>
       </c>
       <c r="U9" s="13">
-        <f t="shared" ref="U9:AE9" si="6">T9/$D9</f>
+        <f t="shared" ref="U9" si="6">T9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="V9" s="23">
+      <c r="V9" s="15">
         <v>0.3</v>
       </c>
       <c r="W9" s="13">
-        <f t="shared" ref="W9:AE9" si="7">V9/$D9</f>
+        <f t="shared" ref="W9" si="7">V9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="X9" s="23">
+      <c r="X9" s="15">
         <v>0.3</v>
       </c>
       <c r="Y9" s="13">
-        <f t="shared" ref="Y9:AE9" si="8">X9/$D9</f>
+        <f t="shared" ref="Y9" si="8">X9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="Z9" s="23">
+      <c r="Z9" s="15">
         <v>0.3</v>
       </c>
       <c r="AA9" s="13">
-        <f t="shared" ref="AA9:AE9" si="9">Z9/$D9</f>
+        <f t="shared" ref="AA9" si="9">Z9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="AB9" s="23">
+      <c r="AB9" s="15">
         <v>0.3</v>
       </c>
       <c r="AC9" s="13">
-        <f t="shared" ref="AC9:AE9" si="10">AB9/$D9</f>
+        <f t="shared" ref="AC9" si="10">AB9/$D9</f>
         <v>1.1538461538461537E-2</v>
       </c>
-      <c r="AD9" s="23">
+      <c r="AD9" s="15">
         <v>0.3</v>
       </c>
       <c r="AE9" s="13">
@@ -1220,93 +1234,83 @@
       </c>
       <c r="E10" s="13">
         <f t="shared" ref="E10:E42" si="12">AVERAGE(G10,I10,K10,M10,O10,Q10,S10,U10,W10,Y10,AA10,AC10,AE10)</f>
-        <v>4.6923076923076949E-2</v>
-      </c>
-      <c r="F10" s="23">
+        <v>5.0000000000000024E-2</v>
+      </c>
+      <c r="F10" s="15">
         <v>1.5</v>
       </c>
       <c r="G10" s="13">
         <f>F10/$D10</f>
         <v>0.15</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="15">
         <v>1.3</v>
       </c>
       <c r="I10" s="13">
         <f>H10/$D10</f>
         <v>0.13</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="15">
         <v>0.3</v>
       </c>
       <c r="K10" s="13">
-        <f t="shared" ref="K10:AE25" si="13">J10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="L10" s="23">
+        <f t="shared" ref="K10:K25" si="13">J10/$D10</f>
+        <v>0.03</v>
+      </c>
+      <c r="L10" s="15">
         <v>0.3</v>
       </c>
       <c r="M10" s="13">
-        <f t="shared" ref="M10:AE25" si="14">L10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="N10" s="23">
+        <f t="shared" ref="M10:M25" si="14">L10/$D10</f>
+        <v>0.03</v>
+      </c>
+      <c r="N10" s="15">
         <v>0.3</v>
       </c>
       <c r="O10" s="13">
-        <f t="shared" ref="O10:AE25" si="15">N10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="P10" s="23">
+        <f t="shared" ref="O10:O25" si="15">N10/$D10</f>
+        <v>0.03</v>
+      </c>
+      <c r="P10" s="15">
         <v>0.3</v>
       </c>
       <c r="Q10" s="13">
-        <f t="shared" ref="Q10:AE25" si="16">P10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="R10" s="23">
+        <f t="shared" ref="Q10:Q25" si="16">P10/$D10</f>
+        <v>0.03</v>
+      </c>
+      <c r="R10" s="15">
         <v>0.3</v>
       </c>
       <c r="S10" s="13">
-        <f t="shared" ref="S10:AE25" si="17">R10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="T10" s="23">
+        <f t="shared" ref="S10:S25" si="17">R10/$D10</f>
+        <v>0.03</v>
+      </c>
+      <c r="T10" s="15">
         <v>0.3</v>
       </c>
       <c r="U10" s="13">
-        <f t="shared" ref="U10:AE25" si="18">T10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="V10" s="23">
+        <f t="shared" ref="U10:U25" si="18">T10/$D10</f>
+        <v>0.03</v>
+      </c>
+      <c r="V10" s="15">
         <v>0.3</v>
       </c>
       <c r="W10" s="13">
-        <f t="shared" ref="W10:AE25" si="19">V10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="X10" s="23">
+        <f t="shared" ref="W10:W25" si="19">V10/$D10</f>
+        <v>0.03</v>
+      </c>
+      <c r="X10" s="15">
         <v>0.3</v>
       </c>
       <c r="Y10" s="13">
-        <f t="shared" ref="Y10:AE25" si="20">X10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="Z10" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA10" s="13">
-        <f t="shared" ref="AA10:AE25" si="21">Z10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="AB10" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC10" s="13">
-        <f t="shared" ref="AC10:AE25" si="22">AB10/$D10</f>
-        <v>0.03</v>
-      </c>
-      <c r="AD10" s="23">
+        <f t="shared" ref="Y10:Y25" si="20">X10/$D10</f>
+        <v>0.03</v>
+      </c>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="25"/>
+      <c r="AD10" s="15">
         <v>0.3</v>
       </c>
       <c r="AE10" s="13">
@@ -1329,93 +1333,83 @@
       </c>
       <c r="E11" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F11" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F11" s="15">
         <v>0.3</v>
       </c>
       <c r="G11" s="13">
-        <f t="shared" ref="G11:G42" si="23">F11/$D11</f>
-        <v>0.03</v>
-      </c>
-      <c r="H11" s="23">
+        <f t="shared" ref="G11:G42" si="21">F11/$D11</f>
+        <v>0.03</v>
+      </c>
+      <c r="H11" s="15">
         <v>0.3</v>
       </c>
       <c r="I11" s="13">
-        <f t="shared" ref="I10:AE25" si="24">H11/$D11</f>
-        <v>0.03</v>
-      </c>
-      <c r="J11" s="23">
+        <f t="shared" ref="I11:I25" si="22">H11/$D11</f>
+        <v>0.03</v>
+      </c>
+      <c r="J11" s="15">
         <v>0.3</v>
       </c>
       <c r="K11" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L11" s="23">
+      <c r="L11" s="15">
         <v>0.3</v>
       </c>
       <c r="M11" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="15">
         <v>0.3</v>
       </c>
       <c r="O11" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P11" s="23">
+      <c r="P11" s="15">
         <v>0.3</v>
       </c>
       <c r="Q11" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="15">
         <v>0.3</v>
       </c>
       <c r="S11" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T11" s="23">
+      <c r="T11" s="15">
         <v>0.3</v>
       </c>
       <c r="U11" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V11" s="23">
+      <c r="V11" s="15">
         <v>0.3</v>
       </c>
       <c r="W11" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X11" s="23">
+      <c r="X11" s="15">
         <v>0.3</v>
       </c>
       <c r="Y11" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z11" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA11" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB11" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC11" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD11" s="23">
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="24"/>
+      <c r="AC11" s="25"/>
+      <c r="AD11" s="15">
         <v>0.3</v>
       </c>
       <c r="AE11" s="13">
@@ -1438,93 +1432,83 @@
       </c>
       <c r="E12" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F12" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F12" s="15">
         <v>0.3</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H12" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H12" s="15">
         <v>0.3</v>
       </c>
       <c r="I12" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J12" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J12" s="15">
         <v>0.3</v>
       </c>
       <c r="K12" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="15">
         <v>0.3</v>
       </c>
       <c r="M12" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="15">
         <v>0.3</v>
       </c>
       <c r="O12" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P12" s="23">
+      <c r="P12" s="15">
         <v>0.3</v>
       </c>
       <c r="Q12" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="15">
         <v>0.3</v>
       </c>
       <c r="S12" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T12" s="23">
+      <c r="T12" s="15">
         <v>0.3</v>
       </c>
       <c r="U12" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V12" s="23">
+      <c r="V12" s="15">
         <v>0.3</v>
       </c>
       <c r="W12" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X12" s="23">
+      <c r="X12" s="15">
         <v>0.3</v>
       </c>
       <c r="Y12" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z12" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA12" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB12" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC12" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD12" s="23">
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="25"/>
+      <c r="AD12" s="15">
         <v>0.3</v>
       </c>
       <c r="AE12" s="13">
@@ -1547,93 +1531,83 @@
       </c>
       <c r="E13" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F13" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F13" s="15">
         <v>0.3</v>
       </c>
       <c r="G13" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H13" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H13" s="15">
         <v>0.3</v>
       </c>
       <c r="I13" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J13" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J13" s="15">
         <v>0.3</v>
       </c>
       <c r="K13" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="15">
         <v>0.3</v>
       </c>
       <c r="M13" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="15">
         <v>0.3</v>
       </c>
       <c r="O13" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P13" s="23">
+      <c r="P13" s="15">
         <v>0.3</v>
       </c>
       <c r="Q13" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R13" s="23">
+      <c r="R13" s="15">
         <v>0.3</v>
       </c>
       <c r="S13" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T13" s="23">
+      <c r="T13" s="15">
         <v>0.3</v>
       </c>
       <c r="U13" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V13" s="23">
+      <c r="V13" s="15">
         <v>0.3</v>
       </c>
       <c r="W13" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X13" s="23">
+      <c r="X13" s="15">
         <v>0.3</v>
       </c>
       <c r="Y13" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z13" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA13" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB13" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC13" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD13" s="23">
+      <c r="Z13" s="24"/>
+      <c r="AA13" s="25"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="25"/>
+      <c r="AD13" s="15">
         <v>0.3</v>
       </c>
       <c r="AE13" s="13">
@@ -1656,93 +1630,83 @@
       </c>
       <c r="E14" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F14" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F14" s="15">
         <v>0.3</v>
       </c>
       <c r="G14" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H14" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H14" s="15">
         <v>0.3</v>
       </c>
       <c r="I14" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J14" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J14" s="15">
         <v>0.3</v>
       </c>
       <c r="K14" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="15">
         <v>0.3</v>
       </c>
       <c r="M14" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="15">
         <v>0.3</v>
       </c>
       <c r="O14" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P14" s="23">
+      <c r="P14" s="15">
         <v>0.3</v>
       </c>
       <c r="Q14" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R14" s="23">
+      <c r="R14" s="15">
         <v>0.3</v>
       </c>
       <c r="S14" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T14" s="23">
+      <c r="T14" s="15">
         <v>0.3</v>
       </c>
       <c r="U14" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V14" s="23">
+      <c r="V14" s="15">
         <v>0.3</v>
       </c>
       <c r="W14" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X14" s="23">
+      <c r="X14" s="15">
         <v>0.3</v>
       </c>
       <c r="Y14" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z14" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA14" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB14" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC14" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD14" s="23">
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="25"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="25"/>
+      <c r="AD14" s="15">
         <v>0.3</v>
       </c>
       <c r="AE14" s="13">
@@ -1765,93 +1729,83 @@
       </c>
       <c r="E15" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F15" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F15" s="15">
         <v>0.3</v>
       </c>
       <c r="G15" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H15" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H15" s="15">
         <v>0.3</v>
       </c>
       <c r="I15" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J15" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J15" s="15">
         <v>0.3</v>
       </c>
       <c r="K15" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L15" s="23">
+      <c r="L15" s="15">
         <v>0.3</v>
       </c>
       <c r="M15" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="15">
         <v>0.3</v>
       </c>
       <c r="O15" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P15" s="23">
+      <c r="P15" s="15">
         <v>0.3</v>
       </c>
       <c r="Q15" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R15" s="23">
+      <c r="R15" s="15">
         <v>0.3</v>
       </c>
       <c r="S15" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T15" s="23">
+      <c r="T15" s="15">
         <v>0.3</v>
       </c>
       <c r="U15" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V15" s="23">
+      <c r="V15" s="15">
         <v>0.3</v>
       </c>
       <c r="W15" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X15" s="23">
+      <c r="X15" s="15">
         <v>0.3</v>
       </c>
       <c r="Y15" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z15" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA15" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB15" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC15" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD15" s="23">
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="25"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="25"/>
+      <c r="AD15" s="15">
         <v>0.3</v>
       </c>
       <c r="AE15" s="13">
@@ -1874,93 +1828,83 @@
       </c>
       <c r="E16" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F16" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F16" s="15">
         <v>0.3</v>
       </c>
       <c r="G16" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H16" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H16" s="15">
         <v>0.3</v>
       </c>
       <c r="I16" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J16" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J16" s="15">
         <v>0.3</v>
       </c>
       <c r="K16" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="15">
         <v>0.3</v>
       </c>
       <c r="M16" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="15">
         <v>0.3</v>
       </c>
       <c r="O16" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P16" s="15">
         <v>0.3</v>
       </c>
       <c r="Q16" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="15">
         <v>0.3</v>
       </c>
       <c r="S16" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T16" s="23">
+      <c r="T16" s="15">
         <v>0.3</v>
       </c>
       <c r="U16" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V16" s="23">
+      <c r="V16" s="15">
         <v>0.3</v>
       </c>
       <c r="W16" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X16" s="23">
+      <c r="X16" s="15">
         <v>0.3</v>
       </c>
       <c r="Y16" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z16" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA16" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB16" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC16" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD16" s="23">
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="25"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="25"/>
+      <c r="AD16" s="15">
         <v>0.3</v>
       </c>
       <c r="AE16" s="13">
@@ -1983,93 +1927,83 @@
       </c>
       <c r="E17" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F17" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F17" s="15">
         <v>0.3</v>
       </c>
       <c r="G17" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H17" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H17" s="15">
         <v>0.3</v>
       </c>
       <c r="I17" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J17" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J17" s="15">
         <v>0.3</v>
       </c>
       <c r="K17" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L17" s="23">
+      <c r="L17" s="15">
         <v>0.3</v>
       </c>
       <c r="M17" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="15">
         <v>0.3</v>
       </c>
       <c r="O17" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P17" s="23">
+      <c r="P17" s="15">
         <v>0.3</v>
       </c>
       <c r="Q17" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R17" s="23">
+      <c r="R17" s="15">
         <v>0.3</v>
       </c>
       <c r="S17" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T17" s="23">
+      <c r="T17" s="15">
         <v>0.3</v>
       </c>
       <c r="U17" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V17" s="23">
+      <c r="V17" s="15">
         <v>0.3</v>
       </c>
       <c r="W17" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X17" s="23">
+      <c r="X17" s="15">
         <v>0.3</v>
       </c>
       <c r="Y17" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z17" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA17" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB17" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC17" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD17" s="23">
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="24"/>
+      <c r="AC17" s="25"/>
+      <c r="AD17" s="15">
         <v>0.3</v>
       </c>
       <c r="AE17" s="13">
@@ -2092,93 +2026,83 @@
       </c>
       <c r="E18" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F18" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F18" s="15">
         <v>0.3</v>
       </c>
       <c r="G18" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H18" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H18" s="15">
         <v>0.3</v>
       </c>
       <c r="I18" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J18" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J18" s="15">
         <v>0.3</v>
       </c>
       <c r="K18" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L18" s="23">
+      <c r="L18" s="15">
         <v>0.3</v>
       </c>
       <c r="M18" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N18" s="15">
         <v>0.3</v>
       </c>
       <c r="O18" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P18" s="23">
+      <c r="P18" s="15">
         <v>0.3</v>
       </c>
       <c r="Q18" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R18" s="23">
+      <c r="R18" s="15">
         <v>0.3</v>
       </c>
       <c r="S18" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T18" s="23">
+      <c r="T18" s="15">
         <v>0.3</v>
       </c>
       <c r="U18" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V18" s="23">
+      <c r="V18" s="15">
         <v>0.3</v>
       </c>
       <c r="W18" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X18" s="23">
+      <c r="X18" s="15">
         <v>0.3</v>
       </c>
       <c r="Y18" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z18" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA18" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB18" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC18" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD18" s="23">
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="25"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="25"/>
+      <c r="AD18" s="15">
         <v>0.3</v>
       </c>
       <c r="AE18" s="13">
@@ -2201,93 +2125,83 @@
       </c>
       <c r="E19" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F19" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F19" s="15">
         <v>0.3</v>
       </c>
       <c r="G19" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H19" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H19" s="15">
         <v>0.3</v>
       </c>
       <c r="I19" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J19" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J19" s="15">
         <v>0.3</v>
       </c>
       <c r="K19" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L19" s="23">
+      <c r="L19" s="15">
         <v>0.3</v>
       </c>
       <c r="M19" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N19" s="15">
         <v>0.3</v>
       </c>
       <c r="O19" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P19" s="23">
+      <c r="P19" s="15">
         <v>0.3</v>
       </c>
       <c r="Q19" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R19" s="23">
+      <c r="R19" s="15">
         <v>0.3</v>
       </c>
       <c r="S19" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T19" s="23">
+      <c r="T19" s="15">
         <v>0.3</v>
       </c>
       <c r="U19" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V19" s="23">
+      <c r="V19" s="15">
         <v>0.3</v>
       </c>
       <c r="W19" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X19" s="23">
+      <c r="X19" s="15">
         <v>0.3</v>
       </c>
       <c r="Y19" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z19" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA19" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB19" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC19" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD19" s="23">
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="25"/>
+      <c r="AB19" s="24"/>
+      <c r="AC19" s="25"/>
+      <c r="AD19" s="15">
         <v>0.3</v>
       </c>
       <c r="AE19" s="13">
@@ -2310,93 +2224,83 @@
       </c>
       <c r="E20" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F20" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F20" s="15">
         <v>0.3</v>
       </c>
       <c r="G20" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H20" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H20" s="15">
         <v>0.3</v>
       </c>
       <c r="I20" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J20" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J20" s="15">
         <v>0.3</v>
       </c>
       <c r="K20" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="15">
         <v>0.3</v>
       </c>
       <c r="M20" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N20" s="23">
+      <c r="N20" s="15">
         <v>0.3</v>
       </c>
       <c r="O20" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P20" s="23">
+      <c r="P20" s="15">
         <v>0.3</v>
       </c>
       <c r="Q20" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R20" s="23">
+      <c r="R20" s="15">
         <v>0.3</v>
       </c>
       <c r="S20" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T20" s="23">
+      <c r="T20" s="15">
         <v>0.3</v>
       </c>
       <c r="U20" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V20" s="23">
+      <c r="V20" s="15">
         <v>0.3</v>
       </c>
       <c r="W20" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X20" s="23">
+      <c r="X20" s="15">
         <v>0.3</v>
       </c>
       <c r="Y20" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z20" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA20" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB20" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC20" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD20" s="23">
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="25"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="25"/>
+      <c r="AD20" s="15">
         <v>0.3</v>
       </c>
       <c r="AE20" s="13">
@@ -2419,93 +2323,83 @@
       </c>
       <c r="E21" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F21" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F21" s="15">
         <v>0.3</v>
       </c>
       <c r="G21" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H21" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H21" s="15">
         <v>0.3</v>
       </c>
       <c r="I21" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J21" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J21" s="15">
         <v>0.3</v>
       </c>
       <c r="K21" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L21" s="23">
+      <c r="L21" s="15">
         <v>0.3</v>
       </c>
       <c r="M21" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N21" s="23">
+      <c r="N21" s="15">
         <v>0.3</v>
       </c>
       <c r="O21" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P21" s="23">
+      <c r="P21" s="15">
         <v>0.3</v>
       </c>
       <c r="Q21" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R21" s="23">
+      <c r="R21" s="15">
         <v>0.3</v>
       </c>
       <c r="S21" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T21" s="23">
+      <c r="T21" s="15">
         <v>0.3</v>
       </c>
       <c r="U21" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V21" s="23">
+      <c r="V21" s="15">
         <v>0.3</v>
       </c>
       <c r="W21" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X21" s="23">
+      <c r="X21" s="15">
         <v>0.3</v>
       </c>
       <c r="Y21" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z21" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA21" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB21" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC21" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD21" s="23">
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="25"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="25"/>
+      <c r="AD21" s="15">
         <v>0.3</v>
       </c>
       <c r="AE21" s="13">
@@ -2528,93 +2422,83 @@
       </c>
       <c r="E22" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F22" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F22" s="15">
         <v>0.3</v>
       </c>
       <c r="G22" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H22" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H22" s="15">
         <v>0.3</v>
       </c>
       <c r="I22" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J22" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J22" s="15">
         <v>0.3</v>
       </c>
       <c r="K22" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L22" s="23">
+      <c r="L22" s="15">
         <v>0.3</v>
       </c>
       <c r="M22" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N22" s="15">
         <v>0.3</v>
       </c>
       <c r="O22" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="15">
         <v>0.3</v>
       </c>
       <c r="Q22" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R22" s="23">
+      <c r="R22" s="15">
         <v>0.3</v>
       </c>
       <c r="S22" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T22" s="23">
+      <c r="T22" s="15">
         <v>0.3</v>
       </c>
       <c r="U22" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V22" s="23">
+      <c r="V22" s="15">
         <v>0.3</v>
       </c>
       <c r="W22" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X22" s="23">
+      <c r="X22" s="15">
         <v>0.3</v>
       </c>
       <c r="Y22" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z22" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA22" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB22" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC22" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD22" s="23">
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="25"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="25"/>
+      <c r="AD22" s="15">
         <v>0.3</v>
       </c>
       <c r="AE22" s="13">
@@ -2637,93 +2521,83 @@
       </c>
       <c r="E23" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F23" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F23" s="15">
         <v>0.3</v>
       </c>
       <c r="G23" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H23" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H23" s="15">
         <v>0.3</v>
       </c>
       <c r="I23" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J23" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J23" s="15">
         <v>0.3</v>
       </c>
       <c r="K23" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L23" s="23">
+      <c r="L23" s="15">
         <v>0.3</v>
       </c>
       <c r="M23" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N23" s="23">
+      <c r="N23" s="15">
         <v>0.3</v>
       </c>
       <c r="O23" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="15">
         <v>0.3</v>
       </c>
       <c r="Q23" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R23" s="23">
+      <c r="R23" s="15">
         <v>0.3</v>
       </c>
       <c r="S23" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T23" s="23">
+      <c r="T23" s="15">
         <v>0.3</v>
       </c>
       <c r="U23" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V23" s="23">
+      <c r="V23" s="15">
         <v>0.3</v>
       </c>
       <c r="W23" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X23" s="23">
+      <c r="X23" s="15">
         <v>0.3</v>
       </c>
       <c r="Y23" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z23" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA23" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB23" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC23" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD23" s="23">
+      <c r="Z23" s="24"/>
+      <c r="AA23" s="25"/>
+      <c r="AB23" s="24"/>
+      <c r="AC23" s="25"/>
+      <c r="AD23" s="15">
         <v>0.3</v>
       </c>
       <c r="AE23" s="13">
@@ -2746,93 +2620,83 @@
       </c>
       <c r="E24" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F24" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F24" s="15">
         <v>0.3</v>
       </c>
       <c r="G24" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H24" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H24" s="15">
         <v>0.3</v>
       </c>
       <c r="I24" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J24" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J24" s="15">
         <v>0.3</v>
       </c>
       <c r="K24" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="15">
         <v>0.3</v>
       </c>
       <c r="M24" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="15">
         <v>0.3</v>
       </c>
       <c r="O24" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P24" s="23">
+      <c r="P24" s="15">
         <v>0.3</v>
       </c>
       <c r="Q24" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R24" s="23">
+      <c r="R24" s="15">
         <v>0.3</v>
       </c>
       <c r="S24" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T24" s="23">
+      <c r="T24" s="15">
         <v>0.3</v>
       </c>
       <c r="U24" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V24" s="23">
+      <c r="V24" s="15">
         <v>0.3</v>
       </c>
       <c r="W24" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X24" s="23">
+      <c r="X24" s="15">
         <v>0.3</v>
       </c>
       <c r="Y24" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z24" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA24" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB24" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC24" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD24" s="23">
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="25"/>
+      <c r="AB24" s="24"/>
+      <c r="AC24" s="25"/>
+      <c r="AD24" s="15">
         <v>0.3</v>
       </c>
       <c r="AE24" s="13">
@@ -2855,93 +2719,83 @@
       </c>
       <c r="E25" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F25" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F25" s="15">
         <v>0.3</v>
       </c>
       <c r="G25" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H25" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H25" s="15">
         <v>0.3</v>
       </c>
       <c r="I25" s="13">
-        <f t="shared" si="24"/>
-        <v>0.03</v>
-      </c>
-      <c r="J25" s="23">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="J25" s="15">
         <v>0.3</v>
       </c>
       <c r="K25" s="13">
         <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
-      <c r="L25" s="23">
+      <c r="L25" s="15">
         <v>0.3</v>
       </c>
       <c r="M25" s="13">
         <f t="shared" si="14"/>
         <v>0.03</v>
       </c>
-      <c r="N25" s="23">
+      <c r="N25" s="15">
         <v>0.3</v>
       </c>
       <c r="O25" s="13">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="P25" s="23">
+      <c r="P25" s="15">
         <v>0.3</v>
       </c>
       <c r="Q25" s="13">
         <f t="shared" si="16"/>
         <v>0.03</v>
       </c>
-      <c r="R25" s="23">
+      <c r="R25" s="15">
         <v>0.3</v>
       </c>
       <c r="S25" s="13">
         <f t="shared" si="17"/>
         <v>0.03</v>
       </c>
-      <c r="T25" s="23">
+      <c r="T25" s="15">
         <v>0.3</v>
       </c>
       <c r="U25" s="13">
         <f t="shared" si="18"/>
         <v>0.03</v>
       </c>
-      <c r="V25" s="23">
+      <c r="V25" s="15">
         <v>0.3</v>
       </c>
       <c r="W25" s="13">
         <f t="shared" si="19"/>
         <v>0.03</v>
       </c>
-      <c r="X25" s="23">
+      <c r="X25" s="15">
         <v>0.3</v>
       </c>
       <c r="Y25" s="13">
         <f t="shared" si="20"/>
         <v>0.03</v>
       </c>
-      <c r="Z25" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA25" s="13">
-        <f t="shared" si="21"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB25" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC25" s="13">
-        <f t="shared" si="22"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD25" s="23">
+      <c r="Z25" s="24"/>
+      <c r="AA25" s="25"/>
+      <c r="AB25" s="24"/>
+      <c r="AC25" s="25"/>
+      <c r="AD25" s="15">
         <v>0.3</v>
       </c>
       <c r="AE25" s="13">
@@ -2964,93 +2818,83 @@
       </c>
       <c r="E26" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F26" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F26" s="15">
         <v>0.3</v>
       </c>
       <c r="G26" s="13">
-        <f t="shared" si="23"/>
-        <v>0.03</v>
-      </c>
-      <c r="H26" s="23">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H26" s="15">
         <v>0.3</v>
       </c>
       <c r="I26" s="13">
-        <f t="shared" ref="I26:I42" si="25">H26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="J26" s="23">
+        <f t="shared" ref="I26:I42" si="23">H26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="J26" s="15">
         <v>0.3</v>
       </c>
       <c r="K26" s="13">
-        <f t="shared" ref="K26:K42" si="26">J26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="L26" s="23">
+        <f t="shared" ref="K26:K42" si="24">J26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="L26" s="15">
         <v>0.3</v>
       </c>
       <c r="M26" s="13">
-        <f t="shared" ref="M26:M42" si="27">L26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="N26" s="23">
+        <f t="shared" ref="M26:M42" si="25">L26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="N26" s="15">
         <v>0.3</v>
       </c>
       <c r="O26" s="13">
-        <f t="shared" ref="O26:O42" si="28">N26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="P26" s="23">
+        <f t="shared" ref="O26:O42" si="26">N26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="P26" s="15">
         <v>0.3</v>
       </c>
       <c r="Q26" s="13">
-        <f t="shared" ref="Q26:Q42" si="29">P26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="R26" s="23">
+        <f t="shared" ref="Q26:Q42" si="27">P26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="R26" s="15">
         <v>0.3</v>
       </c>
       <c r="S26" s="13">
-        <f t="shared" ref="S26:S42" si="30">R26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="T26" s="23">
+        <f t="shared" ref="S26:S42" si="28">R26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="T26" s="15">
         <v>0.3</v>
       </c>
       <c r="U26" s="13">
-        <f t="shared" ref="U26:U42" si="31">T26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="V26" s="23">
+        <f t="shared" ref="U26:U42" si="29">T26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="V26" s="15">
         <v>0.3</v>
       </c>
       <c r="W26" s="13">
-        <f t="shared" ref="W26:W42" si="32">V26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="X26" s="23">
+        <f t="shared" ref="W26:W42" si="30">V26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="X26" s="15">
         <v>0.3</v>
       </c>
       <c r="Y26" s="13">
-        <f t="shared" ref="Y26:Y42" si="33">X26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="Z26" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA26" s="13">
-        <f t="shared" ref="AA26:AA42" si="34">Z26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="AB26" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC26" s="13">
-        <f t="shared" ref="AC26:AC42" si="35">AB26/$D26</f>
-        <v>0.03</v>
-      </c>
-      <c r="AD26" s="23">
+        <f t="shared" ref="Y26:Y42" si="31">X26/$D26</f>
+        <v>0.03</v>
+      </c>
+      <c r="Z26" s="24"/>
+      <c r="AA26" s="25"/>
+      <c r="AB26" s="24"/>
+      <c r="AC26" s="25"/>
+      <c r="AD26" s="15">
         <v>0.3</v>
       </c>
       <c r="AE26" s="13">
@@ -3073,93 +2917,83 @@
       </c>
       <c r="E27" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F27" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F27" s="15">
         <v>0.3</v>
       </c>
       <c r="G27" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I27" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I27" s="13">
+      <c r="J27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K27" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M27" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K27" s="13">
+      <c r="N27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O27" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M27" s="13">
+      <c r="P27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q27" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O27" s="13">
+      <c r="R27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S27" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q27" s="13">
+      <c r="T27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U27" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S27" s="13">
+      <c r="V27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W27" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U27" s="13">
+      <c r="X27" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y27" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W27" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y27" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA27" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB27" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC27" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD27" s="23">
+      <c r="Z27" s="24"/>
+      <c r="AA27" s="25"/>
+      <c r="AB27" s="24"/>
+      <c r="AC27" s="25"/>
+      <c r="AD27" s="15">
         <v>0.3</v>
       </c>
       <c r="AE27" s="13">
@@ -3182,93 +3016,83 @@
       </c>
       <c r="E28" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F28" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F28" s="15">
         <v>0.3</v>
       </c>
       <c r="G28" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I28" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I28" s="13">
+      <c r="J28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K28" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M28" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K28" s="13">
+      <c r="N28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O28" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M28" s="13">
+      <c r="P28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q28" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O28" s="13">
+      <c r="R28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S28" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q28" s="13">
+      <c r="T28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U28" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S28" s="13">
+      <c r="V28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W28" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U28" s="13">
+      <c r="X28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y28" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W28" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y28" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA28" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB28" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC28" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD28" s="23">
+      <c r="Z28" s="24"/>
+      <c r="AA28" s="25"/>
+      <c r="AB28" s="24"/>
+      <c r="AC28" s="25"/>
+      <c r="AD28" s="15">
         <v>0.3</v>
       </c>
       <c r="AE28" s="13">
@@ -3291,93 +3115,83 @@
       </c>
       <c r="E29" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F29" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F29" s="15">
         <v>0.3</v>
       </c>
       <c r="G29" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I29" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I29" s="13">
+      <c r="J29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K29" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M29" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K29" s="13">
+      <c r="N29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O29" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M29" s="13">
+      <c r="P29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q29" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O29" s="13">
+      <c r="R29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S29" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q29" s="13">
+      <c r="T29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U29" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S29" s="13">
+      <c r="V29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W29" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U29" s="13">
+      <c r="X29" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y29" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W29" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y29" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA29" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB29" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC29" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD29" s="23">
+      <c r="Z29" s="24"/>
+      <c r="AA29" s="25"/>
+      <c r="AB29" s="24"/>
+      <c r="AC29" s="25"/>
+      <c r="AD29" s="15">
         <v>0.3</v>
       </c>
       <c r="AE29" s="13">
@@ -3400,93 +3214,83 @@
       </c>
       <c r="E30" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F30" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F30" s="15">
         <v>0.3</v>
       </c>
       <c r="G30" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I30" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I30" s="13">
+      <c r="J30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K30" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M30" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K30" s="13">
+      <c r="N30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O30" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M30" s="13">
+      <c r="P30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q30" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O30" s="13">
+      <c r="R30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S30" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q30" s="13">
+      <c r="T30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U30" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S30" s="13">
+      <c r="V30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W30" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U30" s="13">
+      <c r="X30" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y30" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W30" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y30" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA30" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB30" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC30" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD30" s="23">
+      <c r="Z30" s="24"/>
+      <c r="AA30" s="25"/>
+      <c r="AB30" s="24"/>
+      <c r="AC30" s="25"/>
+      <c r="AD30" s="15">
         <v>0.3</v>
       </c>
       <c r="AE30" s="13">
@@ -3509,93 +3313,83 @@
       </c>
       <c r="E31" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F31" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F31" s="15">
         <v>0.3</v>
       </c>
       <c r="G31" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I31" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I31" s="13">
+      <c r="J31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K31" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M31" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K31" s="13">
+      <c r="N31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O31" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M31" s="13">
+      <c r="P31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q31" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O31" s="13">
+      <c r="R31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S31" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q31" s="13">
+      <c r="T31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U31" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S31" s="13">
+      <c r="V31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W31" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U31" s="13">
+      <c r="X31" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y31" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W31" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y31" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA31" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB31" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC31" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD31" s="23">
+      <c r="Z31" s="24"/>
+      <c r="AA31" s="25"/>
+      <c r="AB31" s="24"/>
+      <c r="AC31" s="25"/>
+      <c r="AD31" s="15">
         <v>0.3</v>
       </c>
       <c r="AE31" s="13">
@@ -3618,93 +3412,83 @@
       </c>
       <c r="E32" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F32" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F32" s="15">
         <v>0.3</v>
       </c>
       <c r="G32" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I32" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I32" s="13">
+      <c r="J32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K32" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M32" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K32" s="13">
+      <c r="N32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O32" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M32" s="13">
+      <c r="P32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q32" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O32" s="13">
+      <c r="R32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S32" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q32" s="13">
+      <c r="T32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U32" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S32" s="13">
+      <c r="V32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W32" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U32" s="13">
+      <c r="X32" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y32" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W32" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y32" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA32" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB32" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC32" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD32" s="23">
+      <c r="Z32" s="24"/>
+      <c r="AA32" s="25"/>
+      <c r="AB32" s="24"/>
+      <c r="AC32" s="25"/>
+      <c r="AD32" s="15">
         <v>0.3</v>
       </c>
       <c r="AE32" s="13">
@@ -3727,93 +3511,83 @@
       </c>
       <c r="E33" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F33" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F33" s="15">
         <v>0.3</v>
       </c>
       <c r="G33" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I33" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I33" s="13">
+      <c r="J33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K33" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M33" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K33" s="13">
+      <c r="N33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O33" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M33" s="13">
+      <c r="P33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q33" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O33" s="13">
+      <c r="R33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S33" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q33" s="13">
+      <c r="T33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U33" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S33" s="13">
+      <c r="V33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W33" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U33" s="13">
+      <c r="X33" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y33" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W33" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y33" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA33" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB33" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC33" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD33" s="23">
+      <c r="Z33" s="24"/>
+      <c r="AA33" s="25"/>
+      <c r="AB33" s="24"/>
+      <c r="AC33" s="25"/>
+      <c r="AD33" s="15">
         <v>0.3</v>
       </c>
       <c r="AE33" s="13">
@@ -3838,91 +3612,91 @@
         <f t="shared" si="12"/>
         <v>3.0000000000000009E-2</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="15">
         <v>0.3</v>
       </c>
       <c r="G34" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I34" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I34" s="13">
+      <c r="J34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K34" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M34" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K34" s="13">
+      <c r="N34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O34" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M34" s="13">
+      <c r="P34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q34" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O34" s="13">
+      <c r="R34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S34" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q34" s="13">
+      <c r="T34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U34" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S34" s="13">
+      <c r="V34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W34" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U34" s="13">
+      <c r="X34" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y34" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W34" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y34" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z34" s="23">
+      <c r="Z34" s="15">
         <v>0.3</v>
       </c>
       <c r="AA34" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB34" s="23">
+        <f t="shared" ref="AA26:AA42" si="32">Z34/$D34</f>
+        <v>0.03</v>
+      </c>
+      <c r="AB34" s="15">
         <v>0.3</v>
       </c>
       <c r="AC34" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD34" s="23">
+        <f t="shared" ref="AC26:AC42" si="33">AB34/$D34</f>
+        <v>0.03</v>
+      </c>
+      <c r="AD34" s="15">
         <v>0.3</v>
       </c>
       <c r="AE34" s="13">
@@ -3947,91 +3721,91 @@
         <f t="shared" si="12"/>
         <v>3.0000000000000009E-2</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="15">
         <v>0.3</v>
       </c>
       <c r="G35" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I35" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I35" s="13">
+      <c r="J35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K35" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M35" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K35" s="13">
+      <c r="N35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O35" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M35" s="13">
+      <c r="P35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q35" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O35" s="13">
+      <c r="R35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S35" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q35" s="13">
+      <c r="T35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U35" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S35" s="13">
+      <c r="V35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W35" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U35" s="13">
+      <c r="X35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y35" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W35" s="13">
+      <c r="Z35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="AA35" s="13">
         <f t="shared" si="32"/>
         <v>0.03</v>
       </c>
-      <c r="X35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y35" s="13">
+      <c r="AB35" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="AC35" s="13">
         <f t="shared" si="33"/>
         <v>0.03</v>
       </c>
-      <c r="Z35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA35" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC35" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD35" s="23">
+      <c r="AD35" s="15">
         <v>0.3</v>
       </c>
       <c r="AE35" s="13">
@@ -4054,93 +3828,83 @@
       </c>
       <c r="E36" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F36" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F36" s="15">
         <v>0.3</v>
       </c>
       <c r="G36" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I36" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I36" s="13">
+      <c r="J36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K36" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M36" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K36" s="13">
+      <c r="N36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O36" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M36" s="13">
+      <c r="P36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q36" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O36" s="13">
+      <c r="R36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S36" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q36" s="13">
+      <c r="T36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U36" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S36" s="13">
+      <c r="V36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W36" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U36" s="13">
+      <c r="X36" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y36" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W36" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y36" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA36" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB36" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC36" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD36" s="23">
+      <c r="Z36" s="24"/>
+      <c r="AA36" s="25"/>
+      <c r="AB36" s="24"/>
+      <c r="AC36" s="25"/>
+      <c r="AD36" s="15">
         <v>0.3</v>
       </c>
       <c r="AE36" s="13">
@@ -4163,93 +3927,83 @@
       </c>
       <c r="E37" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F37" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F37" s="15">
         <v>0.3</v>
       </c>
       <c r="G37" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I37" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I37" s="13">
+      <c r="J37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K37" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M37" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K37" s="13">
+      <c r="N37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O37" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M37" s="13">
+      <c r="P37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q37" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O37" s="13">
+      <c r="R37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S37" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q37" s="13">
+      <c r="T37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U37" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S37" s="13">
+      <c r="V37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W37" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U37" s="13">
+      <c r="X37" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y37" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W37" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y37" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA37" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB37" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC37" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD37" s="23">
+      <c r="Z37" s="24"/>
+      <c r="AA37" s="25"/>
+      <c r="AB37" s="24"/>
+      <c r="AC37" s="25"/>
+      <c r="AD37" s="15">
         <v>0.3</v>
       </c>
       <c r="AE37" s="13">
@@ -4272,93 +4026,83 @@
       </c>
       <c r="E38" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F38" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F38" s="15">
         <v>0.3</v>
       </c>
       <c r="G38" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I38" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I38" s="13">
+      <c r="J38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K38" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M38" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K38" s="13">
+      <c r="N38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O38" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M38" s="13">
+      <c r="P38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q38" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O38" s="13">
+      <c r="R38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S38" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q38" s="13">
+      <c r="T38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U38" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S38" s="13">
+      <c r="V38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W38" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U38" s="13">
+      <c r="X38" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y38" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W38" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y38" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA38" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB38" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC38" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD38" s="23">
+      <c r="Z38" s="24"/>
+      <c r="AA38" s="25"/>
+      <c r="AB38" s="24"/>
+      <c r="AC38" s="25"/>
+      <c r="AD38" s="15">
         <v>0.3</v>
       </c>
       <c r="AE38" s="13">
@@ -4381,93 +4125,83 @@
       </c>
       <c r="E39" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F39" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F39" s="15">
         <v>0.3</v>
       </c>
       <c r="G39" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I39" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I39" s="13">
+      <c r="J39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K39" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M39" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K39" s="13">
+      <c r="N39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O39" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M39" s="13">
+      <c r="P39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q39" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O39" s="13">
+      <c r="R39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S39" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q39" s="13">
+      <c r="T39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U39" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S39" s="13">
+      <c r="V39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W39" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U39" s="13">
+      <c r="X39" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y39" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W39" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y39" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA39" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB39" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC39" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD39" s="23">
+      <c r="Z39" s="24"/>
+      <c r="AA39" s="25"/>
+      <c r="AB39" s="24"/>
+      <c r="AC39" s="25"/>
+      <c r="AD39" s="15">
         <v>0.3</v>
       </c>
       <c r="AE39" s="13">
@@ -4490,93 +4224,83 @@
       </c>
       <c r="E40" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F40" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F40" s="15">
         <v>0.3</v>
       </c>
       <c r="G40" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I40" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I40" s="13">
+      <c r="J40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K40" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M40" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K40" s="13">
+      <c r="N40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O40" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M40" s="13">
+      <c r="P40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q40" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O40" s="13">
+      <c r="R40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S40" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q40" s="13">
+      <c r="T40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U40" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S40" s="13">
+      <c r="V40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W40" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U40" s="13">
+      <c r="X40" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y40" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W40" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y40" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA40" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB40" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC40" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD40" s="23">
+      <c r="Z40" s="24"/>
+      <c r="AA40" s="25"/>
+      <c r="AB40" s="24"/>
+      <c r="AC40" s="25"/>
+      <c r="AD40" s="15">
         <v>0.3</v>
       </c>
       <c r="AE40" s="13">
@@ -4599,93 +4323,83 @@
       </c>
       <c r="E41" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F41" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F41" s="15">
         <v>0.3</v>
       </c>
       <c r="G41" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I41" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I41" s="13">
+      <c r="J41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K41" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M41" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K41" s="13">
+      <c r="N41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O41" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M41" s="13">
+      <c r="P41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q41" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O41" s="13">
+      <c r="R41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S41" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q41" s="13">
+      <c r="T41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U41" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S41" s="13">
+      <c r="V41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W41" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U41" s="13">
+      <c r="X41" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y41" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W41" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y41" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA41" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB41" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC41" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD41" s="23">
+      <c r="Z41" s="24"/>
+      <c r="AA41" s="25"/>
+      <c r="AB41" s="24"/>
+      <c r="AC41" s="25"/>
+      <c r="AD41" s="15">
         <v>0.3</v>
       </c>
       <c r="AE41" s="13">
@@ -4708,93 +4422,83 @@
       </c>
       <c r="E42" s="13">
         <f t="shared" si="12"/>
-        <v>3.0000000000000009E-2</v>
-      </c>
-      <c r="F42" s="23">
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F42" s="15">
         <v>0.3</v>
       </c>
       <c r="G42" s="13">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="H42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="I42" s="13">
         <f t="shared" si="23"/>
         <v>0.03</v>
       </c>
-      <c r="H42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="I42" s="13">
+      <c r="J42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="K42" s="13">
+        <f t="shared" si="24"/>
+        <v>0.03</v>
+      </c>
+      <c r="L42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M42" s="13">
         <f t="shared" si="25"/>
         <v>0.03</v>
       </c>
-      <c r="J42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="K42" s="13">
+      <c r="N42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="O42" s="13">
         <f t="shared" si="26"/>
         <v>0.03</v>
       </c>
-      <c r="L42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="M42" s="13">
+      <c r="P42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Q42" s="13">
         <f t="shared" si="27"/>
         <v>0.03</v>
       </c>
-      <c r="N42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="O42" s="13">
+      <c r="R42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="S42" s="13">
         <f t="shared" si="28"/>
         <v>0.03</v>
       </c>
-      <c r="P42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Q42" s="13">
+      <c r="T42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U42" s="13">
         <f t="shared" si="29"/>
         <v>0.03</v>
       </c>
-      <c r="R42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="S42" s="13">
+      <c r="V42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="W42" s="13">
         <f t="shared" si="30"/>
         <v>0.03</v>
       </c>
-      <c r="T42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="U42" s="13">
+      <c r="X42" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="Y42" s="13">
         <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
-      <c r="V42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="W42" s="13">
-        <f t="shared" si="32"/>
-        <v>0.03</v>
-      </c>
-      <c r="X42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="Y42" s="13">
-        <f t="shared" si="33"/>
-        <v>0.03</v>
-      </c>
-      <c r="Z42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AA42" s="13">
-        <f t="shared" si="34"/>
-        <v>0.03</v>
-      </c>
-      <c r="AB42" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AC42" s="13">
-        <f t="shared" si="35"/>
-        <v>0.03</v>
-      </c>
-      <c r="AD42" s="23">
+      <c r="Z42" s="24"/>
+      <c r="AA42" s="25"/>
+      <c r="AB42" s="24"/>
+      <c r="AC42" s="25"/>
+      <c r="AD42" s="15">
         <v>0.3</v>
       </c>
       <c r="AE42" s="13">
@@ -7675,11 +7379,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="AE6:AE7"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="AB6:AC6"/>
     <mergeCell ref="P5:Y5"/>
     <mergeCell ref="Z5:AC5"/>
     <mergeCell ref="AD5:AE5"/>
@@ -7696,11 +7400,11 @@
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="Z6:AA6"/>
     <mergeCell ref="AD6:AD7"/>
-    <mergeCell ref="AE6:AE7"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E42">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>